<commit_message>
Clase 13 de junio:recursion parte 2
</commit_message>
<xml_diff>
--- a/Semana 9/Recursion.xlsx
+++ b/Semana 9/Recursion.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiacortes/Desktop/P1Q22024/Semana 9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408F732C-2079-9E43-AC57-A60C26083F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F09CA2-F56A-EC44-A32D-998755A95263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="740" windowWidth="15000" windowHeight="18900" activeTab="2" xr2:uid="{6BA569F9-AE5B-9745-9897-42971319989A}"/>
+    <workbookView xWindow="15240" yWindow="760" windowWidth="15000" windowHeight="17180" activeTab="3" xr2:uid="{6BA569F9-AE5B-9745-9897-42971319989A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Prueba de Escritorio" sheetId="3" r:id="rId3"/>
+    <sheet name="Prueba de escritorio buscar " sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t>1. El factorial solamente se calcula a numeros positivos, o sea &gt;= 0</t>
   </si>
@@ -247,10 +248,13 @@
     <t xml:space="preserve">4. la computadora, solo se puede enfocar en una cosa a la vez </t>
   </si>
   <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Cda vez que podamos hacer return, va a ser como sacar un libro de la caja </t>
+    <t xml:space="preserve">5. Cada vez que podamos hacer return, va a ser como sacar un libro de la caja </t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main   , encontro_recursivo = false </t>
   </si>
 </sst>
 </file>
@@ -304,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -327,27 +331,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,7 +824,7 @@
   <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,13 +833,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -800,12 +852,12 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -966,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F784FAA-A28E-7C4C-B623-1F081D2BEACE}">
   <dimension ref="C2:L20"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A4" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,35 +1113,35 @@
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="F12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="F13" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
       <c r="F14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
       <c r="H15" t="s">
         <v>57</v>
       </c>
@@ -1101,8 +1153,8 @@
       </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
       <c r="F16" t="s">
         <v>53</v>
       </c>
@@ -1114,19 +1166,19 @@
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
       <c r="F17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="F19" t="s">
         <v>55</v>
       </c>
@@ -1149,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5A63EE-C67E-CE49-A095-548BD6476405}">
   <dimension ref="A2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A2" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,80 +1216,169 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="204" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
+      <c r="B11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="8"/>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B16" s="8"/>
+      <c r="B16" s="6"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E994F3-5E67-6A4B-A109-2067C99E702E}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="260" zoomScaleNormal="260" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>